<commit_message>
implemented window and fixed short window, also debug pyomo opt mode
</commit_message>
<xml_diff>
--- a/tests/integration_tests/workflows/storage/analytic.xlsx
+++ b/tests/integration_tests/workflows/storage/analytic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/talbpw/projects/HERON/tests/integration_tests/storage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/talbpw/projects/HERON/tests/integration_tests/workflows/storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AD3C8A-87D3-C347-A486-92D550495BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796562EA-2AEC-814E-8CBC-097A4F14B12E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80860" yWindow="12780" windowWidth="43240" windowHeight="17440" activeTab="1" xr2:uid="{D0FB268D-148C-FA40-8069-E11220FC7D23}"/>
+    <workbookView xWindow="0" yWindow="26260" windowWidth="43240" windowHeight="17440" xr2:uid="{D0FB268D-148C-FA40-8069-E11220FC7D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Case 1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -520,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E9901-C9EE-9948-846C-E17303C6B6B5}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,7 +831,7 @@
         <v>0.2</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" ref="J10:W10" si="1">I10+0.1</f>
+        <f t="shared" ref="J10:O10" si="1">I10+0.1</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="K10" s="6">
@@ -1997,7 +2000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A39E27-8097-774F-8230-3D9ED6209ECF}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tests pass, no _or_ charge option, but working
</commit_message>
<xml_diff>
--- a/tests/integration_tests/workflows/storage/analytic.xlsx
+++ b/tests/integration_tests/workflows/storage/analytic.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/talbpw/projects/HERON/tests/integration_tests/workflows/storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796562EA-2AEC-814E-8CBC-097A4F14B12E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA151DF6-4CEF-AA41-8D91-37103F55142E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="26260" windowWidth="43240" windowHeight="17440" xr2:uid="{D0FB268D-148C-FA40-8069-E11220FC7D23}"/>
+    <workbookView xWindow="36060" yWindow="10400" windowWidth="34480" windowHeight="17440" activeTab="1" xr2:uid="{D0FB268D-148C-FA40-8069-E11220FC7D23}"/>
   </bookViews>
   <sheets>
-    <sheet name="Case 1" sheetId="2" r:id="rId1"/>
-    <sheet name="Case 2" sheetId="1" r:id="rId2"/>
+    <sheet name="Case 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Case 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Case 1 no RTE" sheetId="2" r:id="rId3"/>
+    <sheet name="Case 2 no RTE" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="39">
   <si>
     <t>ARMA Signal</t>
   </si>
@@ -137,6 +139,21 @@
   </si>
   <si>
     <t>Note the Steamer is making more steam than the Generator can possibly convert into electricity. The Storage is used to mitigate large expenses in the end of the history.</t>
+  </si>
+  <si>
+    <t>RTE</t>
+  </si>
+  <si>
+    <t>charge</t>
+  </si>
+  <si>
+    <t>discharge</t>
+  </si>
+  <si>
+    <t>balance check</t>
+  </si>
+  <si>
+    <t>loss this step</t>
   </si>
 </sst>
 </file>
@@ -520,11 +537,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E9901-C9EE-9948-846C-E17303C6B6B5}">
-  <dimension ref="A1:Y36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C8283F-2323-B442-ABA2-E776AB3DB5CE}">
+  <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,6 +558,9 @@
       <c r="B1" t="s">
         <v>26</v>
       </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -549,6 +569,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -772,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="Y8">
-        <f t="shared" ref="Y8:Y22" si="0">SUM(C8:W8)</f>
+        <f t="shared" ref="Y8:Y23" si="0">SUM(C8:W8)</f>
         <v>21</v>
       </c>
     </row>
@@ -824,6 +847,3225 @@
         <v>0</v>
       </c>
       <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+      <c r="R10" s="6">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6">
+        <v>0</v>
+      </c>
+      <c r="X10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <f>-(D10-C10)/0.1</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" ref="E11:W11" si="1">-(E10-D10)/0.1</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6">
+        <v>9.4868330000000007</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0</v>
+      </c>
+      <c r="R12" s="6">
+        <v>0</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0</v>
+      </c>
+      <c r="T12" s="6">
+        <v>0</v>
+      </c>
+      <c r="U12" s="6">
+        <v>0</v>
+      </c>
+      <c r="V12" s="6">
+        <v>0</v>
+      </c>
+      <c r="W12" s="6">
+        <v>0</v>
+      </c>
+      <c r="X12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-10.486833000000001</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="R14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="S14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="T14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="V14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="W14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>-30.486833000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.2434165000000004</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>15.2434165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="L17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="M17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="N17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="O17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="P17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="R17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="S17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="T17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="U17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="V17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="W17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4">
+        <f>C18*C17*-1</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" ref="D19:W19" si="2">D18*D17*-1</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="R19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="S19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="T19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="V19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="W19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-5.2434165000000004</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="0"/>
+        <v>-7.2434165000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3">
+        <f>-2*(C6-0.5)</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" ref="D22:W22" si="3">-2*(D6-0.5)</f>
+        <v>0.87441895999999997</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.74933353200000008</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.62523737000000001</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.502620226</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.38196601200000002</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.26375089399999996</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.14844141600000005</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="3"/>
+        <v>3.6492651999999959E-2</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="3"/>
+        <v>-7.1653589999999934E-2</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.17557050399999996</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.2748479800000001</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.36909421200000003</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.45793725399999996</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.54102648600000003</v>
+      </c>
+      <c r="R22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.61803398800000009</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.6886558519999999</v>
+      </c>
+      <c r="T22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.75261336000000001</v>
+      </c>
+      <c r="U22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.80965410400000004</v>
+      </c>
+      <c r="V22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.85955297199999992</v>
+      </c>
+      <c r="W22" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.90211303199999993</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="0"/>
+        <v>-1.9384922719999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4">
+        <f>C22*C21*-1</f>
+        <v>5.2434165000000004</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" ref="D23:W23" si="4">D22*D21*-1</f>
+        <v>0.43720947999999998</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="4"/>
+        <v>0.37466676600000004</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="4"/>
+        <v>0.31261868500000001</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="4"/>
+        <v>0.251310113</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="0"/>
+        <v>6.6192215440000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:W27" si="5">C23+C19</f>
+        <v>5.2434165000000004</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="5"/>
+        <v>0.43720947999999998</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>0.37466676600000004</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>0.31261868500000001</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>0.251310113</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" ref="Y27:Y29" si="6">SUM(C27:W27)</f>
+        <v>10.619221544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <f>C8+C14+C11+C12</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:W28" si="7">D8+D14+D11</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <f>C21+C17+C15</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:W29" si="8">D21+D17+D15</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>Y27</f>
+        <v>10.619221544</v>
+      </c>
+      <c r="D36">
+        <f>Y27</f>
+        <v>10.619221544</v>
+      </c>
+      <c r="E36">
+        <f>Y27</f>
+        <v>10.619221544</v>
+      </c>
+      <c r="G36">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="5">
+        <f>NPV(G36,C36:E36) + B36</f>
+        <v>27.366763847960165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BA86E-B1DA-6D45-84AD-44BAD7E84500}">
+  <dimension ref="A1:Y39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>0.6</v>
+      </c>
+      <c r="J5">
+        <v>0.7</v>
+      </c>
+      <c r="K5">
+        <v>0.8</v>
+      </c>
+      <c r="L5">
+        <v>0.9</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O5">
+        <v>1.2</v>
+      </c>
+      <c r="P5">
+        <v>1.3</v>
+      </c>
+      <c r="Q5">
+        <v>1.4</v>
+      </c>
+      <c r="R5">
+        <v>1.5</v>
+      </c>
+      <c r="S5">
+        <v>1.6</v>
+      </c>
+      <c r="T5">
+        <v>1.7</v>
+      </c>
+      <c r="U5">
+        <v>1.8</v>
+      </c>
+      <c r="V5">
+        <v>1.9</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6.2790520000000002E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.12533323399999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.18738131499999999</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.248689887</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.30901699399999999</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.36812455300000002</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.42577929199999998</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.48175367400000002</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.53582679499999997</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.58778525199999998</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.63742399000000005</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.68454710600000002</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.72896862699999998</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.77051324300000001</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.80901699400000004</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.84432792599999995</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0.87630668</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.90482705200000002</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.92977648599999996</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.95105651599999996</v>
+      </c>
+      <c r="Y6">
+        <f>SUM(C6:W6)</f>
+        <v>11.469246136000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>100</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>100</v>
+      </c>
+      <c r="F8" s="2">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2">
+        <v>100</v>
+      </c>
+      <c r="H8" s="2">
+        <v>100</v>
+      </c>
+      <c r="I8" s="2">
+        <v>100</v>
+      </c>
+      <c r="J8" s="2">
+        <v>100</v>
+      </c>
+      <c r="K8" s="2">
+        <v>100</v>
+      </c>
+      <c r="L8" s="2">
+        <v>100</v>
+      </c>
+      <c r="M8" s="2">
+        <v>100</v>
+      </c>
+      <c r="N8" s="2">
+        <v>100</v>
+      </c>
+      <c r="O8" s="2">
+        <v>100</v>
+      </c>
+      <c r="P8" s="2">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>100</v>
+      </c>
+      <c r="R8" s="2">
+        <v>100</v>
+      </c>
+      <c r="S8" s="2">
+        <v>100</v>
+      </c>
+      <c r="T8" s="2">
+        <v>100</v>
+      </c>
+      <c r="U8" s="2">
+        <v>100</v>
+      </c>
+      <c r="V8" s="2">
+        <v>100</v>
+      </c>
+      <c r="W8" s="2">
+        <v>100</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ref="Y8:Y25" si="0">SUM(C8:W8)</f>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+      <c r="R10" s="6">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6">
+        <v>9.1073596999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-104.86833</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="I11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="J11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="K11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="L11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="M11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="N11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="O11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="P11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="R11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="S11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="T11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="U11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="V11" s="6">
+        <v>-960</v>
+      </c>
+      <c r="W11" s="6">
+        <v>-96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6">
+        <v>103.86833</v>
+      </c>
+      <c r="D12" s="6">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9</v>
+      </c>
+      <c r="F12" s="6">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6">
+        <v>9</v>
+      </c>
+      <c r="H12" s="6">
+        <v>9</v>
+      </c>
+      <c r="I12" s="6">
+        <v>9</v>
+      </c>
+      <c r="J12" s="6">
+        <v>9</v>
+      </c>
+      <c r="K12" s="6">
+        <v>9</v>
+      </c>
+      <c r="L12" s="6">
+        <v>864</v>
+      </c>
+      <c r="M12" s="6">
+        <v>864</v>
+      </c>
+      <c r="N12" s="6">
+        <v>864</v>
+      </c>
+      <c r="O12" s="6">
+        <v>864</v>
+      </c>
+      <c r="P12" s="6">
+        <v>864</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>864</v>
+      </c>
+      <c r="R12" s="6">
+        <v>864</v>
+      </c>
+      <c r="S12" s="6">
+        <v>864</v>
+      </c>
+      <c r="T12" s="6">
+        <v>864</v>
+      </c>
+      <c r="U12" s="6">
+        <v>864</v>
+      </c>
+      <c r="V12" s="6">
+        <v>864</v>
+      </c>
+      <c r="W12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6">
+        <f>(C10-A11)/0.1 + C11*SQRT(F2) + C12/SQRT(F2)</f>
+        <v>2.0549393298097129E-8</v>
+      </c>
+      <c r="D13" s="6">
+        <f>(D10-C10)/0.1 + D11*SQRT($F$2) + D12/SQRT($F$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" ref="E13:W13" si="1">(E10-D10)/0.1 + E11*SQRT($F$2) + E12/SQRT($F$2)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="6">
+        <f t="shared" si="1"/>
+        <v>3.8715067773864575E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="6">
+        <f>(ABS(C11)+ABS(C12))*SQRT($F$2)*0.1</f>
+        <v>19.802498303284878</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" ref="D14:W14" si="2">(ABS(D11)+ABS(D12))*SQRT($F$2)*0.1</f>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8024982662959763</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="Q14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="R14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="S14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="T14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="U14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="V14" s="6">
+        <f t="shared" si="2"/>
+        <v>173.03983356441373</v>
+      </c>
+      <c r="W14" s="6">
+        <f t="shared" si="2"/>
+        <v>9.1073596612849315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="H16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="I16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="J16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="K16" s="2">
+        <v>-99</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="M16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="N16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="O16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="P16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="R16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="S16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="T16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="U16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="V16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="W16" s="2">
+        <v>-4</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="0"/>
+        <v>-939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="L17" s="1">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>2</v>
+      </c>
+      <c r="N17" s="1">
+        <v>2</v>
+      </c>
+      <c r="O17" s="1">
+        <v>2</v>
+      </c>
+      <c r="P17" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>2</v>
+      </c>
+      <c r="S17" s="1">
+        <v>2</v>
+      </c>
+      <c r="T17" s="1">
+        <v>2</v>
+      </c>
+      <c r="U17" s="1">
+        <v>2</v>
+      </c>
+      <c r="V17" s="1">
+        <v>2</v>
+      </c>
+      <c r="W17" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="0"/>
+        <v>469.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="K19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="L19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="M19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="N19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="R19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="S19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="T19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="U19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="V19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="W19" s="1">
+        <v>-2</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="0"/>
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4">
+        <f>C20*C19*-1</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" ref="D21:W21" si="3">D20*D19*-1</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-49.5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-49.5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-49.5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-49.5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-49.5</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-47.5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-47.5</v>
+      </c>
+      <c r="J23" s="1">
+        <v>-47.5</v>
+      </c>
+      <c r="K23" s="1">
+        <v>-47.5</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="0"/>
+        <v>-437.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <f>-2*(C6-0.5)</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24:W24" si="4">-2*(D6-0.5)</f>
+        <v>0.87441895999999997</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.74933353200000008</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.62523737000000001</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.502620226</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.38196601200000002</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.26375089399999996</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.14844141600000005</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="4"/>
+        <v>3.6492651999999959E-2</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="4"/>
+        <v>-7.1653589999999934E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.17557050399999996</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.2748479800000001</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.36909421200000003</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.45793725399999996</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.54102648600000003</v>
+      </c>
+      <c r="R24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.61803398800000009</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.6886558519999999</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.75261336000000001</v>
+      </c>
+      <c r="U24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.80965410400000004</v>
+      </c>
+      <c r="V24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.85955297199999992</v>
+      </c>
+      <c r="W24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.90211303199999993</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="0"/>
+        <v>-1.9384922719999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4">
+        <f>C24*C23*-1</f>
+        <v>49.5</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" ref="D25:W25" si="5">D24*D23*-1</f>
+        <v>43.28373852</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="5"/>
+        <v>37.092009834000002</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="5"/>
+        <v>30.949249815000002</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="5"/>
+        <v>24.879701186999998</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="5"/>
+        <v>18.14338557</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="5"/>
+        <v>12.528167464999997</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="5"/>
+        <v>7.050967260000002</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="5"/>
+        <v>1.7334009699999982</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="0"/>
+        <v>225.16062062099996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:W29" si="6">C25+C21</f>
+        <v>49.5</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="6"/>
+        <v>43.28373852</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="6"/>
+        <v>37.092009834000002</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="6"/>
+        <v>30.949249815000002</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>24.879701186999998</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="6"/>
+        <v>19.14338557</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>13.528167464999997</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="6"/>
+        <v>8.050967260000002</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>2.7334009699999982</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Y31" si="7">SUM(C29:W29)</f>
+        <v>241.16062062099996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f>C8+C16+C12+C11</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:W30" si="8">D8+D16+D12+D11</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f>C23+C19+C17</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:W31" si="9">D23+D19+D17</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>Y29</f>
+        <v>241.16062062099996</v>
+      </c>
+      <c r="D38">
+        <f>Y29</f>
+        <v>241.16062062099996</v>
+      </c>
+      <c r="E38">
+        <f>Y29</f>
+        <v>241.16062062099996</v>
+      </c>
+      <c r="G38">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="5">
+        <f>NPV(G38,C38:E38) + B38</f>
+        <v>621.49430884520757</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E9901-C9EE-9948-846C-E17303C6B6B5}">
+  <dimension ref="A1:Y36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:W16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="3.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>0.6</v>
+      </c>
+      <c r="J5">
+        <v>0.7</v>
+      </c>
+      <c r="K5">
+        <v>0.8</v>
+      </c>
+      <c r="L5">
+        <v>0.9</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O5">
+        <v>1.2</v>
+      </c>
+      <c r="P5">
+        <v>1.3</v>
+      </c>
+      <c r="Q5">
+        <v>1.4</v>
+      </c>
+      <c r="R5">
+        <v>1.5</v>
+      </c>
+      <c r="S5">
+        <v>1.6</v>
+      </c>
+      <c r="T5">
+        <v>1.7</v>
+      </c>
+      <c r="U5">
+        <v>1.8</v>
+      </c>
+      <c r="V5">
+        <v>1.9</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6.2790520000000002E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.12533323399999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.18738131499999999</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.248689887</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.30901699399999999</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.36812455300000002</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.42577929199999998</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.48175367400000002</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.53582679499999997</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.58778525199999998</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.63742399000000005</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.68454710600000002</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.72896862699999998</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.77051324300000001</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.80901699400000004</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.84432792599999995</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0.87630668</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.90482705200000002</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.92977648599999996</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.95105651599999996</v>
+      </c>
+      <c r="Y6">
+        <f>SUM(C6:W6)</f>
+        <v>11.469246136000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ref="Y8:Y22" si="0">SUM(C8:W8)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
         <v>0.1</v>
       </c>
       <c r="I10" s="6">
@@ -1996,7 +5238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A39E27-8097-774F-8230-3D9ED6209ECF}">
   <dimension ref="A1:Y36"/>
   <sheetViews>

</xml_diff>